<commit_message>
Ready to do parallelism
</commit_message>
<xml_diff>
--- a/miscellenaous/estimation of time.xlsx
+++ b/miscellenaous/estimation of time.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YoupiYoupin\Documents\GitHub\g-unit-of-agreement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YoupiYoupin\Documents\GitHub\g-unit-of-agreement\miscellenaous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD5C6C1-BB49-4ED8-87A9-6DCE1F7ADBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF911C3-D246-4F62-B606-0931B7DA18E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32580" yWindow="2910" windowWidth="21600" windowHeight="11295" xr2:uid="{51D91FD6-07AF-4AC4-84DD-83503357D3FD}"/>
+    <workbookView xWindow="33795" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{51D91FD6-07AF-4AC4-84DD-83503357D3FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="speed" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <r>
       <t>2E-05x</t>
@@ -49,6 +50,12 @@
       </rPr>
       <t>2.9502</t>
     </r>
+  </si>
+  <si>
+    <t>difference in resolution</t>
+  </si>
+  <si>
+    <t>150x150 matrix</t>
   </si>
 </sst>
 </file>
@@ -112,351 +119,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$6:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>550</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>600</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$6:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AB98-4B69-AC78-1D584C4F058A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="386313328"/>
-        <c:axId val="386314576"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="386313328"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="386314576"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="386314576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="386313328"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -577,7 +239,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$14</c:f>
+              <c:f>speed!$A$1:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -628,7 +290,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$14</c:f>
+              <c:f>speed!$B$1:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -871,6 +533,736 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>speed!$C$1:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>speed!$E$1:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.30579237503246992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0114189457094189</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3633353183507286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5648789507629539</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8168139927959821</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.265183447987802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.279949826049204</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.735259510716823</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.41273129910914</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76.503910869693243</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.199548720323023</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>116.68966452794965</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>141.16360204927025</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>168.81007649521555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>199.81721581999332</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>272.66327829361512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C79E-4A94-943D-99385394CD9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1560525823"/>
+        <c:axId val="1560527071"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1560525823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1560527071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1560527071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1560525823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0454934546075601E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.169999543132034</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.237977307194498</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.386353899356844</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.79492558678967096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0006759661868301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1702351958566699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4478231037960199</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9840219616961301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-64FA-4CBD-AECE-77CABF6BF4D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1363465391"/>
+        <c:axId val="1536978703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1363465391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1536978703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1536978703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1363465391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -951,6 +1343,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1983,27 +2415,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7545C021-7024-47A7-B58B-487FECD643D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7136B063-2B91-A7DE-9448-44E88A59A787}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2023,23 +2971,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7136B063-2B91-A7DE-9448-44E88A59A787}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1FA11FE-EC82-3DCE-D9E7-2644B5DEE7A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2052,6 +3000,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C7D92EE-4CC6-593F-D7FD-62D103F97B08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2357,15 +3346,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407EC9DB-A709-4BED-A3D0-388AC0FF255E}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -2379,8 +3368,18 @@
         <f>0.00002*(C1^(2.9502))</f>
         <v>15.901203501688437</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <f>D1/52</f>
+        <v>0.30579237503246992</v>
+      </c>
+      <c r="Q1">
+        <v>30</v>
+      </c>
+      <c r="R1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>150</v>
       </c>
@@ -2391,14 +3390,32 @@
         <v>150</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D16" si="0">0.00002*(C2^(2.9502))</f>
+        <f t="shared" ref="D2:D17" si="0">0.00002*(C2^(2.9502))</f>
         <v>52.593785176889789</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E17" si="1">D2/52</f>
+        <v>1.0114189457094189</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <f>O2*20</f>
+        <v>45.217391304347821</v>
+      </c>
+      <c r="O2">
+        <f>52/23</f>
+        <v>2.2608695652173911</v>
+      </c>
+      <c r="Q2">
+        <v>150</v>
+      </c>
+      <c r="R2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -2412,8 +3429,12 @@
         <f t="shared" si="0"/>
         <v>122.89343655423788</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" si="1"/>
+        <v>2.3633353183507286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>250</v>
       </c>
@@ -2427,8 +3448,12 @@
         <f t="shared" si="0"/>
         <v>237.37370543967361</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>4.5648789507629539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>300</v>
       </c>
@@ -2442,8 +3467,12 @@
         <f t="shared" si="0"/>
         <v>406.47432762539108</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>7.8168139927959821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>400</v>
       </c>
@@ -2457,8 +3486,12 @@
         <f t="shared" si="0"/>
         <v>949.78953929536578</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>18.265183447987802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>500</v>
       </c>
@@ -2472,8 +3505,15 @@
         <f t="shared" si="0"/>
         <v>1834.5573909545587</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f>D7/52</f>
+        <v>35.279949826049204</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>550</v>
       </c>
@@ -2487,8 +3527,12 @@
         <f t="shared" si="0"/>
         <v>2430.2334945572748</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>46.735259510716823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>600</v>
       </c>
@@ -2502,8 +3546,12 @@
         <f t="shared" si="0"/>
         <v>3141.4620275536754</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>60.41273129910914</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>650</v>
       </c>
@@ -2517,8 +3565,12 @@
         <f t="shared" si="0"/>
         <v>3978.2033652240484</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>76.503910869693243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>700</v>
       </c>
@@ -2532,8 +3584,12 @@
         <f t="shared" si="0"/>
         <v>4950.376533456797</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>95.199548720323023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>750</v>
       </c>
@@ -2547,8 +3603,12 @@
         <f t="shared" si="0"/>
         <v>6067.8625554533819</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>116.68966452794965</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>800</v>
       </c>
@@ -2562,8 +3622,12 @@
         <f t="shared" si="0"/>
         <v>7340.5073065620527</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>141.16360204927025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>850</v>
       </c>
@@ -2577,23 +3641,429 @@
         <f t="shared" si="0"/>
         <v>8778.1239777512092</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>168.81007649521555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C15">
-        <v>10000</v>
+        <v>900</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>12642413.64010543</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10390.495222639653</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>199.81721581999332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C16">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>11272753116.519152</v>
+        <v>14178.490471267985</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>272.66327829361512</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>10000</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>12642413.64010543</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>243123.33923279674</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>D16/32</f>
+        <v>443.07782722712454</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>D16/24</f>
+        <v>590.77043630283276</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2911F046-EFE2-4BE1-8E69-E59149F71F3A}">
+  <dimension ref="A1:J42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>500</v>
+      </c>
+      <c r="B4">
+        <v>3.0454934546075601E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>0.169999543132034</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>0.237977307194498</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>0.386353899356844</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>0.79492558678967096</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>1.0006759661868301</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1.1702351958566699</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2.4478231037960199</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>4.9840219616961301</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>75</v>
+      </c>
+      <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <v>25</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>15</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>100</v>
+      </c>
+      <c r="B24">
+        <f>0.00002*(A24^(2.9502))</f>
+        <v>15.901203501688437</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>150</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:B39" si="0">0.00002*(A25^(2.9502))</f>
+        <v>52.593785176889789</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>200</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>122.89343655423788</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>250</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>237.37370543967361</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>300</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>406.47432762539108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>400</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>949.78953929536578</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>500</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>1834.5573909545587</v>
+      </c>
+      <c r="C30">
+        <v>815</v>
+      </c>
+      <c r="D30">
+        <v>485</v>
+      </c>
+      <c r="E30">
+        <v>230</v>
+      </c>
+      <c r="F30">
+        <v>72</v>
+      </c>
+      <c r="G30">
+        <v>55</v>
+      </c>
+      <c r="H30">
+        <v>36</v>
+      </c>
+      <c r="I30">
+        <v>27</v>
+      </c>
+      <c r="J30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>550</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>2430.2334945572748</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>600</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>3141.4620275536754</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>650</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>3978.2033652240484</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>700</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>4950.376533456797</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>750</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>6067.8625554533819</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>800</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>7340.5073065620527</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>850</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>8778.1239777512092</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>900</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>10390.495222639653</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1000</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>14178.490471267985</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>B30/H30</f>
+        <v>50.959927526515521</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>B30/G30</f>
+        <v>33.355588926446522</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f>53/1.5</f>
+        <v>35.333333333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ready to import to python
</commit_message>
<xml_diff>
--- a/miscellenaous/estimation of time.xlsx
+++ b/miscellenaous/estimation of time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YoupiYoupin\Documents\GitHub\g-unit-of-agreement\miscellenaous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF911C3-D246-4F62-B606-0931B7DA18E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C601CD-20DB-483E-B4B7-7021403813D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33795" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{51D91FD6-07AF-4AC4-84DD-83503357D3FD}"/>
+    <workbookView xWindow="2475" yWindow="1440" windowWidth="21600" windowHeight="11295" xr2:uid="{51D91FD6-07AF-4AC4-84DD-83503357D3FD}"/>
   </bookViews>
   <sheets>
     <sheet name="speed" sheetId="1" r:id="rId1"/>
@@ -3348,8 +3348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407EC9DB-A709-4BED-A3D0-388AC0FF255E}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3707,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2911F046-EFE2-4BE1-8E69-E59149F71F3A}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
WORK ON g_oxy LIB NOW
</commit_message>
<xml_diff>
--- a/miscellenaous/estimation of time.xlsx
+++ b/miscellenaous/estimation of time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YoupiYoupin\Documents\GitHub\g-unit-of-agreement\miscellenaous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C601CD-20DB-483E-B4B7-7021403813D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF396379-604F-4B3C-99FA-36F4B4BEA2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2475" yWindow="1440" windowWidth="21600" windowHeight="11295" xr2:uid="{51D91FD6-07AF-4AC4-84DD-83503357D3FD}"/>
   </bookViews>
@@ -3349,7 +3349,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>